<commit_message>
docs: 1. Recalculate the formula for debts for the second worksheet. 2. Allow debts name or owner to be editable.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="5435" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBBABF65-7FBB-4F69-A265-FA05BF34BE37}"/>
+  <xr:revisionPtr revIDLastSave="5517" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCB81B1B-4685-4626-BEAA-66870E1F9B7F}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3064" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="119">
   <si>
     <t>Money In Terms Of</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>17th April 2025</t>
+  </si>
+  <si>
+    <t>Social Welfare</t>
   </si>
   <si>
     <t>03th May 2025</t>
@@ -10885,7 +10888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E410128-C7AA-4335-9548-8A1FBFF72764}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
@@ -11210,7 +11213,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -11386,7 +11389,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -13757,6 +13760,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -14197,7 +14201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70450F9-E58B-48E7-B2C3-C3B422FBA5BC}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A92" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:G40"/>
     </sheetView>
   </sheetViews>
@@ -14523,7 +14527,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -14699,7 +14703,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -17070,6 +17074,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -17510,7 +17515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A615ABE1-ED79-40A7-958D-4E58DAAE3045}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -17834,7 +17839,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -18010,7 +18015,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -20381,6 +20386,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -20821,7 +20827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628B5D1C-A1EA-4FDF-B055-77B4FFDAC151}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
@@ -21147,7 +21153,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -21323,7 +21329,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -23694,6 +23700,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -24134,7 +24141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02693470-7D0F-49B7-A05A-4A71D50C16FE}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
@@ -24458,7 +24465,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -24634,7 +24641,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -27006,6 +27013,7 @@
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
     <protectedRange sqref="A68:C74" name="F4"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A189:B189"/>
@@ -27446,7 +27454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D63BC2C-F2EB-411B-940E-2EFD2713E71D}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:G28"/>
     </sheetView>
   </sheetViews>
@@ -27770,7 +27778,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -27946,7 +27954,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -30317,6 +30325,7 @@
     <protectedRange sqref="A117" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A189:B189"/>
@@ -30757,7 +30766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA65ECD-1234-4154-84AE-122A6F6A70C2}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -31081,7 +31090,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -31257,7 +31266,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -33628,6 +33637,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A189:B189"/>
@@ -34068,7 +34078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5037C0-2D2A-4A46-895F-C10C72C6DE43}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="G180" sqref="G180"/>
     </sheetView>
   </sheetViews>
@@ -34394,7 +34404,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -34570,7 +34580,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -36941,6 +36951,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A189:B189"/>
@@ -37381,8 +37392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40533,7 +40544,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="F12" sqref="F12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40681,12 +40692,10 @@
         <v>115</v>
       </c>
       <c r="B10" s="155" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="C10" s="155"/>
-      <c r="D10" s="155" t="s">
-        <v>51</v>
-      </c>
+      <c r="D10" s="155"/>
       <c r="E10" s="155"/>
       <c r="F10" s="150">
         <v>0</v>
@@ -40854,7 +40863,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -41030,7 +41039,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -41992,6 +42001,7 @@
       </c>
       <c r="B98" s="19"/>
       <c r="C98" s="28">
+        <f>(((Forecast_1!E131+Forecast_1!E158+Forecast_1!E185))+SUM(E118+E145+E172))-Forecast_1!C112</f>
         <v>0</v>
       </c>
       <c r="D98" s="44"/>
@@ -42007,7 +42017,7 @@
       </c>
       <c r="B99" s="19"/>
       <c r="C99" s="28">
-        <f>(((Forecast_1!E132+Forecast_1!E159+Forecast_1!E186))-SUM(E119+E146+E173))-Forecast_1!C113</f>
+        <f>(((Forecast_1!E132+Forecast_1!E159+Forecast_1!E186))+SUM(E119+E146+E173))-Forecast_1!C113</f>
         <v>0</v>
       </c>
       <c r="D99" s="44"/>
@@ -42023,6 +42033,7 @@
       </c>
       <c r="B100" s="19"/>
       <c r="C100" s="28">
+        <f>(((Forecast_1!E133+Forecast_1!E160+Forecast_1!E187))+SUM(E120+E147+E174))-Forecast_1!C114</f>
         <v>0</v>
       </c>
       <c r="D100" s="44"/>
@@ -42038,7 +42049,7 @@
       </c>
       <c r="B101" s="19"/>
       <c r="C101" s="28">
-        <f>((((Forecast_1!E134+Forecast_1!E161+Forecast_1!E188)))-SUM(E121+E148+E175))-Forecast_1!C115</f>
+        <f>((((Forecast_1!E134+Forecast_1!E161+Forecast_1!E188)))+SUM(E121+E148+E175))-Forecast_1!C115</f>
         <v>0</v>
       </c>
       <c r="D101" s="44"/>
@@ -42070,7 +42081,7 @@
       </c>
       <c r="B103" s="19"/>
       <c r="C103" s="28">
-        <f>((((Forecast_1!E136+Forecast_1!E163+Forecast_1!E190)))-SUM(E123+E150+E177))-Forecast_1!C117</f>
+        <f>((((Forecast_1!E136+Forecast_1!E163+Forecast_1!E190)))+SUM(E123+E150+E177))-Forecast_1!C117</f>
         <v>0</v>
       </c>
       <c r="D103" s="44"/>
@@ -42086,7 +42097,7 @@
       </c>
       <c r="B104" s="19"/>
       <c r="C104" s="28">
-        <f>((((Forecast_1!E137+Forecast_1!E164+Forecast_1!E190)))-SUM(E124+E151+E178))-Forecast_1!C118</f>
+        <f>((((Forecast_1!E137+Forecast_1!E164+Forecast_1!E190)))+SUM(E124+E151+E178))-Forecast_1!C118</f>
         <v>0</v>
       </c>
       <c r="D104" s="44"/>
@@ -42102,7 +42113,7 @@
       </c>
       <c r="B105" s="19"/>
       <c r="C105" s="28">
-        <f>((((Forecast_1!E138+Forecast_1!E165+Forecast_1!E192)))-SUM(E125+E152+E179))-Forecast_1!C119</f>
+        <f>((((Forecast_1!E138+Forecast_1!E165+Forecast_1!E192)))+SUM(E125+E152+E179))-Forecast_1!C119</f>
         <v>0</v>
       </c>
       <c r="D105" s="44"/>
@@ -42118,7 +42129,7 @@
       </c>
       <c r="B106" s="19"/>
       <c r="C106" s="28">
-        <f>((((Forecast_1!E139+Forecast_1!E166+Forecast_1!E193)))-SUM(E126+E153+E180))-Forecast_1!C120</f>
+        <f>((((Forecast_1!E139+Forecast_1!E166+Forecast_1!E193)))+SUM(E126+E153+E180))-Forecast_1!C120</f>
         <v>0</v>
       </c>
       <c r="D106" s="44"/>
@@ -42134,7 +42145,7 @@
       </c>
       <c r="B107" s="19"/>
       <c r="C107" s="28">
-        <f>((((Forecast_1!E140+Forecast_1!E167+Forecast_1!E194)))-SUM(E127+E154+E181))-Forecast_1!C121</f>
+        <f>((((Forecast_1!E140+Forecast_1!E167+Forecast_1!E194)))+SUM(E127+E154+E181))-Forecast_1!C121</f>
         <v>0</v>
       </c>
       <c r="D107" s="44"/>
@@ -43378,6 +43389,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="173">
     <mergeCell ref="C172:D172"/>
@@ -43807,8 +43819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0194D17C-96EB-4FD2-8587-7E7A0672619C}">
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44127,7 +44139,7 @@
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -44303,7 +44315,7 @@
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -46653,6 +46665,7 @@
     <protectedRange sqref="A67:C74" name="F3"/>
     <protectedRange sqref="A76:C84" name="F4"/>
     <protectedRange sqref="A86:C94" name="F5"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="C173:D173"/>
@@ -47073,7 +47086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DB7BA1-7701-4FD8-AB09-F7645F43CF33}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A83" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -47398,7 +47411,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -47574,7 +47587,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -49945,6 +49958,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A106" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -50385,7 +50399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57149C74-5589-4903-8EFC-FFF56B2CB1C8}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A84" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:G40"/>
     </sheetView>
   </sheetViews>
@@ -50711,7 +50725,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -50887,7 +50901,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -53258,6 +53272,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -53698,8 +53713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893696C1-98C3-4F01-A415-90003CF2A311}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:G28"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54022,7 +54037,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -54198,7 +54213,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -56569,6 +56584,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A22:G28" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -57009,7 +57025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDDCB6F-10E3-4F34-B456-81FA80F60BFA}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -57333,7 +57349,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -57509,7 +57525,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -59880,6 +59896,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>
@@ -60320,7 +60337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F450479-C751-4C53-A2ED-EE5DA60A80DD}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A81" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
@@ -60645,7 +60662,7 @@
     </row>
     <row r="22" spans="1:9" ht="24.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="155" t="s">
         <v>54</v>
@@ -60821,7 +60838,7 @@
     </row>
     <row r="34" spans="1:9" ht="24.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="155" t="s">
         <v>54</v>
@@ -63192,6 +63209,7 @@
     <protectedRange sqref="C117:E134" name="E1"/>
     <protectedRange sqref="C144:E161" name="E2"/>
     <protectedRange sqref="C171:E188" name="E3"/>
+    <protectedRange sqref="A98:A107" name="D1"/>
   </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A5:B5"/>

</xml_diff>

<commit_message>
docs: 1. Protect cover page.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="2"/>
+    <workbookView windowHeight="21560"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -2377,8 +2377,8 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:Z62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="17.6"/>
@@ -4124,6 +4124,7 @@
       <c r="Z62" s="175"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:Z31"/>
     <mergeCell ref="A32:Z62"/>
@@ -31884,8 +31885,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:G26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34725,7 +34726,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
docs: 1. Formated Cell.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560"/>
+    <workbookView windowHeight="21560" firstSheet="4" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -1584,7 +1584,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1733,11 +1733,11 @@
     <xf numFmtId="178" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2377,7 +2377,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
@@ -4139,7 +4139,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -4883,7 +4883,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -5029,7 +5029,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -5149,7 +5149,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -5282,7 +5282,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -5415,7 +5415,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -5431,7 +5431,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -5600,7 +5600,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -5616,7 +5616,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -7161,7 +7161,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -7905,7 +7905,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -8051,7 +8051,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -8171,7 +8171,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -8304,7 +8304,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -8437,7 +8437,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -8453,7 +8453,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -8622,7 +8622,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="42" t="s">
+      <c r="B108" s="93" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -8638,7 +8638,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="42" t="s">
+      <c r="B109" s="93" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -10183,7 +10183,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -10928,7 +10928,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -11074,7 +11074,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -11194,7 +11194,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -11327,7 +11327,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -11460,7 +11460,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -11476,7 +11476,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -11645,7 +11645,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -11661,7 +11661,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -13206,7 +13206,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -13949,7 +13949,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -14095,7 +14095,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -14215,7 +14215,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -14348,7 +14348,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -14481,7 +14481,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -14497,7 +14497,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -14666,7 +14666,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -14682,7 +14682,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -16227,7 +16227,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -16972,7 +16972,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -17105,7 +17105,7 @@
     </row>
     <row r="65" ht="24.75" customHeight="1" spans="1:9">
       <c r="A65" s="35"/>
-      <c r="B65" s="93"/>
+      <c r="B65" s="92"/>
       <c r="C65" s="37">
         <v>0</v>
       </c>
@@ -17118,7 +17118,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -17238,7 +17238,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -17371,7 +17371,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -17504,7 +17504,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -17520,7 +17520,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -17689,7 +17689,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -17705,7 +17705,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -19250,7 +19250,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -19993,7 +19993,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -20139,7 +20139,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -20259,7 +20259,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -20392,7 +20392,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -20525,7 +20525,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -20541,7 +20541,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -20710,7 +20710,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -20726,7 +20726,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -22272,7 +22272,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -23015,7 +23015,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -23161,7 +23161,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -23281,7 +23281,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -23414,7 +23414,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -23547,7 +23547,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -23563,7 +23563,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -23732,7 +23732,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -23748,7 +23748,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -25293,7 +25293,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -26036,7 +26036,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -26182,7 +26182,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -26302,7 +26302,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -26435,7 +26435,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -26568,7 +26568,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -26584,7 +26584,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -26753,7 +26753,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -26769,7 +26769,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -28314,8 +28314,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -30920,7 +30920,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -31885,8 +31885,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A52" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -33107,7 +33107,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="41"/>
-      <c r="B69" s="92" t="s">
+      <c r="B69" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C69" s="126">
@@ -33326,7 +33326,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="52"/>
-      <c r="B99" s="92" t="s">
+      <c r="B99" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C99" s="37">
@@ -33399,7 +33399,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="40"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C109" s="126">
@@ -33409,7 +33409,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="52"/>
-      <c r="B110" s="92" t="s">
+      <c r="B110" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C110" s="126">
@@ -34726,8 +34726,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35467,7 +35467,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -35613,7 +35613,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -35733,7 +35733,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -35866,7 +35866,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -35999,7 +35999,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -36015,7 +36015,7 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -36184,7 +36184,7 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="94">
@@ -36200,7 +36200,7 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="94">
@@ -37715,7 +37715,7 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A161" workbookViewId="0">
+    <sheetView topLeftCell="A81" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
@@ -38454,7 +38454,7 @@
     </row>
     <row r="55" ht="30" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -38600,7 +38600,7 @@
     </row>
     <row r="66" ht="30" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -38720,7 +38720,7 @@
     </row>
     <row r="75" ht="30" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -38853,7 +38853,7 @@
     </row>
     <row r="85" ht="30" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -38986,7 +38986,7 @@
     </row>
     <row r="95" ht="30" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -39002,7 +39002,7 @@
     </row>
     <row r="96" ht="30" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -39171,7 +39171,7 @@
     </row>
     <row r="108" ht="30" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -39187,7 +39187,7 @@
     </row>
     <row r="109" ht="30" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -40695,7 +40695,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -41439,7 +41439,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -41585,7 +41585,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -41705,7 +41705,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -41838,7 +41838,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -41971,7 +41971,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -41987,7 +41987,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -42156,7 +42156,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -42172,7 +42172,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -43717,8 +43717,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116:D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44462,7 +44462,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -44608,7 +44608,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -44728,7 +44728,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -44861,7 +44861,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -44994,7 +44994,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -45010,7 +45010,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -45179,7 +45179,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="37">
@@ -45195,7 +45195,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="37">
@@ -46740,7 +46740,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -47483,7 +47483,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -47629,7 +47629,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -47749,7 +47749,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -47882,7 +47882,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -48015,7 +48015,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -48031,7 +48031,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -48200,7 +48200,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="94">
@@ -48216,7 +48216,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="94">
@@ -49761,8 +49761,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50504,7 +50504,7 @@
     </row>
     <row r="55" ht="24.75" customHeight="1" spans="1:9">
       <c r="A55" s="41"/>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="37">
@@ -50650,7 +50650,7 @@
     </row>
     <row r="66" ht="24.75" customHeight="1" spans="1:9">
       <c r="A66" s="52"/>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="37">
@@ -50770,7 +50770,7 @@
     </row>
     <row r="75" ht="24.75" customHeight="1" spans="1:9">
       <c r="A75" s="52"/>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C75" s="37">
@@ -50903,7 +50903,7 @@
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C85" s="37">
@@ -51036,7 +51036,7 @@
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:9">
       <c r="A95" s="40"/>
-      <c r="B95" s="92" t="s">
+      <c r="B95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C95" s="37">
@@ -51052,7 +51052,7 @@
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:9">
       <c r="A96" s="52"/>
-      <c r="B96" s="92" t="s">
+      <c r="B96" s="42" t="s">
         <v>53</v>
       </c>
       <c r="C96" s="37">
@@ -51221,7 +51221,7 @@
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:9">
       <c r="A108" s="52"/>
-      <c r="B108" s="92" t="s">
+      <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C108" s="94">
@@ -51237,7 +51237,7 @@
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:9">
       <c r="A109" s="52"/>
-      <c r="B109" s="92" t="s">
+      <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="94">

</xml_diff>

<commit_message>
docs: Changed Money in terms of Label.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" firstSheet="4" activeTab="17"/>
+    <workbookView windowHeight="21560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -74,10 +74,11 @@
     <t>Your Personal Finance Organizer</t>
   </si>
   <si>
-    <t>Money In Terms Of</t>
+    <t>Money In Terms Of
+(tens, hundred, thousands, millions)</t>
   </si>
   <si>
-    <t>-</t>
+    <t>tens</t>
   </si>
   <si>
     <t>A Month</t>
@@ -28314,7 +28315,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="B108" sqref="B108:B109"/>
     </sheetView>
   </sheetViews>
@@ -31337,8 +31338,8 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
@@ -31849,7 +31850,7 @@
     <row r="133" s="153" customFormat="1" ht="20.25" customHeight="1"/>
     <row r="134" s="153" customFormat="1" ht="20.25" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" objects="1"/>
+  <sheetProtection formatCells="0"/>
   <protectedRanges>
     <protectedRange sqref="B1:B6" name="Settings"/>
     <protectedRange sqref="B9:B56" name="NameOfWorkSheet"/>

</xml_diff>

<commit_message>
docs: Set to Cover page.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="1"/>
+    <workbookView windowHeight="21560"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -2378,7 +2378,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
@@ -31338,7 +31338,7 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
docs: 1. Protected Worksheet. 2. Set to Cover Page.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="1"/>
+    <workbookView windowHeight="21560"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Forecast_4" sheetId="5" r:id="rId6"/>
     <sheet name="Forecast_5" sheetId="6" r:id="rId7"/>
     <sheet name="Forecast_6" sheetId="7" r:id="rId8"/>
-    <sheet name="October 2026 - November 2026" sheetId="8" r:id="rId9"/>
+    <sheet name="Forecast_7" sheetId="8" r:id="rId9"/>
     <sheet name="Forecast_8" sheetId="9" r:id="rId10"/>
     <sheet name="Forecast_9" sheetId="10" r:id="rId11"/>
     <sheet name="Forecast_10" sheetId="11" r:id="rId12"/>
@@ -2378,7 +2378,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
@@ -4189,9 +4189,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4205,9 +4205,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4221,9 +4221,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -5462,9 +5462,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -5476,9 +5476,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -5490,9 +5490,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -5504,9 +5504,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -5518,9 +5518,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -5532,9 +5532,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -5546,9 +5546,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -5560,9 +5560,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -5574,9 +5574,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -5588,9 +5588,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -5604,9 +5604,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -5620,9 +5620,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -5714,9 +5714,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -5982,9 +5982,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -6074,9 +6074,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -6342,9 +6342,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -6434,9 +6434,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -6702,9 +6702,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -6745,7 +6745,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -7211,9 +7211,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -7227,9 +7227,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7243,9 +7243,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -8484,9 +8484,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -8498,9 +8498,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -8512,9 +8512,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -8526,9 +8526,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -8540,9 +8540,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -8554,9 +8554,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -8568,9 +8568,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -8582,9 +8582,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -8596,9 +8596,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -8610,9 +8610,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -8626,9 +8626,9 @@
       <c r="B108" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -8642,9 +8642,9 @@
       <c r="B109" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -8736,9 +8736,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -9004,9 +9004,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -9096,9 +9096,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -9364,9 +9364,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -9456,9 +9456,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -9724,9 +9724,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9767,7 +9767,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -10234,9 +10234,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -10250,9 +10250,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10266,9 +10266,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -11507,9 +11507,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -11521,9 +11521,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -11535,9 +11535,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -11549,9 +11549,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -11563,9 +11563,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -11577,9 +11577,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -11591,9 +11591,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -11605,9 +11605,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -11619,9 +11619,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -11633,9 +11633,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -11649,9 +11649,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -11665,9 +11665,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -11759,9 +11759,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -12027,9 +12027,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -12119,9 +12119,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -12387,9 +12387,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -12479,9 +12479,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -12747,9 +12747,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12790,7 +12790,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -13255,9 +13255,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -13271,9 +13271,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -13287,9 +13287,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -14528,9 +14528,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -14542,9 +14542,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -14556,9 +14556,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -14570,9 +14570,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -14584,9 +14584,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -14598,9 +14598,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -14612,9 +14612,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -14626,9 +14626,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -14640,9 +14640,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -14654,9 +14654,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -14670,9 +14670,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -14686,9 +14686,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -14780,9 +14780,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -15048,9 +15048,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -15140,9 +15140,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -15408,9 +15408,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15500,9 +15500,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15768,9 +15768,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15811,7 +15811,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -16278,9 +16278,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -16294,9 +16294,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16310,9 +16310,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -17551,9 +17551,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -17565,9 +17565,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -17579,9 +17579,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -17593,9 +17593,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -17607,9 +17607,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -17621,9 +17621,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -17635,9 +17635,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -17649,9 +17649,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -17663,9 +17663,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -17677,9 +17677,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -17693,9 +17693,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -17709,9 +17709,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -17803,9 +17803,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18071,9 +18071,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18163,9 +18163,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18431,9 +18431,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18523,9 +18523,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18791,9 +18791,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18834,7 +18834,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -19299,9 +19299,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19315,9 +19315,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19331,9 +19331,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -20572,9 +20572,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -20586,9 +20586,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -20600,9 +20600,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -20614,9 +20614,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -20628,9 +20628,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -20642,9 +20642,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -20656,9 +20656,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -20670,9 +20670,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -20684,9 +20684,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -20698,9 +20698,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -20714,9 +20714,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -20730,9 +20730,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -20824,9 +20824,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21092,9 +21092,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21184,9 +21184,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21452,9 +21452,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21544,9 +21544,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21812,9 +21812,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21856,7 +21856,7 @@
     </row>
     <row r="194" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -22321,9 +22321,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22337,9 +22337,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22353,9 +22353,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -23594,9 +23594,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -23608,9 +23608,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -23622,9 +23622,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -23636,9 +23636,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -23650,9 +23650,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -23664,9 +23664,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -23678,9 +23678,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -23692,9 +23692,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -23706,9 +23706,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -23720,9 +23720,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -23736,9 +23736,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -23752,9 +23752,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -23846,9 +23846,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24114,9 +24114,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24206,9 +24206,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24474,9 +24474,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24566,9 +24566,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24834,9 +24834,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -24877,7 +24877,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -25342,9 +25342,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25358,9 +25358,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25374,9 +25374,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -26615,9 +26615,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -26629,9 +26629,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -26643,9 +26643,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -26657,9 +26657,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -26671,9 +26671,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -26685,9 +26685,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -26699,9 +26699,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -26713,9 +26713,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -26727,9 +26727,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -26741,9 +26741,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -26757,9 +26757,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -26773,9 +26773,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -26867,9 +26867,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -27135,9 +27135,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27227,9 +27227,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27495,9 +27495,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27587,9 +27587,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27855,9 +27855,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -27898,7 +27898,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -28315,8 +28315,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126:D126"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -28365,9 +28365,9 @@
       <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="e">
+      <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28381,9 +28381,9 @@
         <v>42</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="e">
+      <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28397,9 +28397,9 @@
         <v>64</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="e">
+      <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -29638,9 +29638,9 @@
     <row r="98" ht="24.75" customHeight="1" spans="1:9">
       <c r="A98" s="40"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="37" t="e" cm="1">
+      <c r="C98" s="37" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="69"/>
@@ -29652,9 +29652,9 @@
     <row r="99" ht="24.75" customHeight="1" spans="1:9">
       <c r="A99" s="40"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="37" t="e" cm="1">
+      <c r="C99" s="37" cm="1">
         <f ca="1" t="array" ref="C99">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C99")+SUM(E119+E146+E173)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -29666,9 +29666,9 @@
     <row r="100" ht="24.75" customHeight="1" spans="1:9">
       <c r="A100" s="40"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="37" t="e" cm="1">
+      <c r="C100" s="37" cm="1">
         <f ca="1" t="array" ref="C100">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C100")+SUM(E120+E147+E174)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -29680,9 +29680,9 @@
     <row r="101" ht="24.75" customHeight="1" spans="1:9">
       <c r="A101" s="35"/>
       <c r="B101" s="36"/>
-      <c r="C101" s="37" t="e" cm="1">
+      <c r="C101" s="37" cm="1">
         <f ca="1" t="array" ref="C101">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C101")+SUM(E121+E148+E175)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
@@ -29694,9 +29694,9 @@
     <row r="102" ht="24.75" customHeight="1" spans="1:9">
       <c r="A102" s="35"/>
       <c r="B102" s="36"/>
-      <c r="C102" s="37" t="e" cm="1">
+      <c r="C102" s="37" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C102")+SUM(E122+E149+E176)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
@@ -29708,9 +29708,9 @@
     <row r="103" ht="24.75" customHeight="1" spans="1:9">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
-      <c r="C103" s="37" t="e" cm="1">
+      <c r="C103" s="37" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -29722,9 +29722,9 @@
     <row r="104" ht="24.75" customHeight="1" spans="1:9">
       <c r="A104" s="35"/>
       <c r="B104" s="36"/>
-      <c r="C104" s="37" t="e" cm="1">
+      <c r="C104" s="37" cm="1">
         <f ca="1" t="array" ref="C104">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C104")+SUM(E124+E151+E178)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
@@ -29736,9 +29736,9 @@
     <row r="105" ht="24.75" customHeight="1" spans="1:9">
       <c r="A105" s="35"/>
       <c r="B105" s="36"/>
-      <c r="C105" s="37" t="e" cm="1">
+      <c r="C105" s="37" cm="1">
         <f ca="1" t="array" ref="C105">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C105")+SUM(E125+E152+E179)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -29750,9 +29750,9 @@
     <row r="106" ht="24.75" customHeight="1" spans="1:9">
       <c r="A106" s="35"/>
       <c r="B106" s="36"/>
-      <c r="C106" s="37" t="e" cm="1">
+      <c r="C106" s="37" cm="1">
         <f ca="1" t="array" ref="C106">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C106")+SUM(E126+E153+E180)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -29764,9 +29764,9 @@
     <row r="107" ht="24.75" customHeight="1" spans="1:9">
       <c r="A107" s="35"/>
       <c r="B107" s="36"/>
-      <c r="C107" s="37" t="e" cm="1">
+      <c r="C107" s="37" cm="1">
         <f ca="1" t="array" ref="C107">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C107")+SUM(E127+E154+E181)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -29780,9 +29780,9 @@
       <c r="B108" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="37" t="e">
+      <c r="C108" s="37">
         <f ca="1">SUM(C98:C107)</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -29796,9 +29796,9 @@
       <c r="B109" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C109" s="37" t="e">
+      <c r="C109" s="37">
         <f ca="1">C108-C96</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -29890,9 +29890,9 @@
       <c r="B116" s="57"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
-      <c r="E116" s="71" t="e" cm="1">
+      <c r="E116" s="71" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30158,9 +30158,9 @@
         <v>61</v>
       </c>
       <c r="D136" s="82"/>
-      <c r="E136" s="88" t="e">
+      <c r="E136" s="88">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30250,9 +30250,9 @@
       <c r="B143" s="57"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
-      <c r="E143" s="88" t="e">
+      <c r="E143" s="88">
         <f ca="1">E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30518,9 +30518,9 @@
         <v>61</v>
       </c>
       <c r="D163" s="82"/>
-      <c r="E163" s="91" t="e">
+      <c r="E163" s="91">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30610,9 +30610,9 @@
       <c r="B170" s="57"/>
       <c r="C170" s="58"/>
       <c r="D170" s="58"/>
-      <c r="E170" s="91" t="e">
+      <c r="E170" s="91">
         <f ca="1">E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -30878,9 +30878,9 @@
         <v>61</v>
       </c>
       <c r="D190" s="82"/>
-      <c r="E190" s="91" t="e">
+      <c r="E190" s="91">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -30921,7 +30921,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -31338,7 +31338,7 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -32175,7 +32175,7 @@
         <v>11 October 2026 - 10 January 2027</v>
       </c>
       <c r="N9" s="144">
-        <f ca="1">'October 2026 - November 2026'!C5</f>
+        <f ca="1">Forecast_7!C5</f>
         <v>0</v>
       </c>
     </row>
@@ -32206,9 +32206,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
         <v>11 January 2027 - 10 April 2027</v>
       </c>
-      <c r="N10" s="135" t="e">
+      <c r="N10" s="135">
         <f ca="1">Forecast_8!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" spans="1:14">
@@ -32235,9 +32235,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
         <v>11 April 2027 - 10 July 2027</v>
       </c>
-      <c r="N11" s="139" t="e">
+      <c r="N11" s="139">
         <f ca="1">Forecast_9!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" spans="1:14">
@@ -32263,9 +32263,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
         <v>11 July 2027 - 10 October 2027</v>
       </c>
-      <c r="N12" s="139" t="e">
+      <c r="N12" s="139">
         <f ca="1">Forecast_10!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" spans="1:14">
@@ -32291,9 +32291,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
         <v>11 October 2027 - 10 January 2028</v>
       </c>
-      <c r="N13" s="139" t="e">
+      <c r="N13" s="139">
         <f ca="1">Forecast_11!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="35.25" customHeight="1" spans="1:14">
@@ -32319,9 +32319,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
         <v>11 January 2028 - 10 April 2028</v>
       </c>
-      <c r="N14" s="139" t="e">
+      <c r="N14" s="139">
         <f ca="1">Forecast_12!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" spans="1:14">
@@ -32347,9 +32347,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
         <v>11 April 2028 - 10 July 2028</v>
       </c>
-      <c r="N15" s="139" t="e">
+      <c r="N15" s="139">
         <f ca="1">Forecast_13!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="35.25" customHeight="1" spans="1:14">
@@ -32381,9 +32381,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
         <v>11 July 2028 - 10 October 2028</v>
       </c>
-      <c r="N16" s="139" t="e">
+      <c r="N16" s="139">
         <f ca="1">Forecast_14!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" ht="35.25" customHeight="1" spans="9:14">
@@ -32399,9 +32399,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
         <v>11 October 2028 - 10 January 2029</v>
       </c>
-      <c r="N17" s="139" t="e">
+      <c r="N17" s="139">
         <f ca="1">Forecast_15!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" ht="35.25" customHeight="1" spans="9:14">
@@ -32417,9 +32417,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
         <v>11 January 2029 - 10 April 2029</v>
       </c>
-      <c r="N18" s="135" t="e">
+      <c r="N18" s="135">
         <f ca="1">Forecast_16!C5</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="33" customHeight="1" spans="9:10">
@@ -32448,7 +32448,7 @@
         <v>11 October 2026 - 10 November 2026</v>
       </c>
       <c r="J21" s="139">
-        <f ca="1">'October 2026 - November 2026'!E136</f>
+        <f ca="1">Forecast_7!E136</f>
         <v>0</v>
       </c>
     </row>
@@ -32468,7 +32468,7 @@
         <v>11 November 2026 - 10 December 2026</v>
       </c>
       <c r="J22" s="139">
-        <f ca="1">'October 2026 - November 2026'!E163</f>
+        <f ca="1">Forecast_7!E163</f>
         <v>0</v>
       </c>
     </row>
@@ -32493,7 +32493,7 @@
         <v>11 December 2026 - 10 January 2027</v>
       </c>
       <c r="J23" s="139">
-        <f ca="1">'October 2026 - November 2026'!E190</f>
+        <f ca="1">Forecast_7!E190</f>
         <v>0</v>
       </c>
     </row>
@@ -32511,9 +32511,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21)+21,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,22)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*22+21),"dd mmmm yyyy"))</f>
         <v>11 January 2027 - 10 February 2027</v>
       </c>
-      <c r="J24" s="139" t="e">
+      <c r="J24" s="139">
         <f ca="1">Forecast_8!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -32530,9 +32530,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,22),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*22)+22,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,23)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*23+22),"dd mmmm yyyy"))</f>
         <v>11 February 2027 - 10 March 2027</v>
       </c>
-      <c r="J25" s="139" t="e">
+      <c r="J25" s="139">
         <f ca="1">Forecast_8!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -32549,9 +32549,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,23),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*23)+23,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
         <v>11 March 2027 - 10 April 2027</v>
       </c>
-      <c r="J26" s="139" t="e">
+      <c r="J26" s="139">
         <f ca="1">Forecast_8!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -32568,9 +32568,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24)+24,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,25)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*25+24),"dd mmmm yyyy"))</f>
         <v>11 April 2027 - 10 May 2027</v>
       </c>
-      <c r="J27" s="139" t="e">
+      <c r="J27" s="139">
         <f ca="1">Forecast_9!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -32587,9 +32587,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,25),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*25)+25,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,26)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*26+25),"dd mmmm yyyy"))</f>
         <v>11 May 2027 - 10 June 2027</v>
       </c>
-      <c r="J28" s="139" t="e">
+      <c r="J28" s="139">
         <f ca="1">Forecast_9!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -32606,9 +32606,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,26),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*26)+26,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
         <v>11 June 2027 - 10 July 2027</v>
       </c>
-      <c r="J29" s="135" t="e">
+      <c r="J29" s="135">
         <f ca="1">Forecast_9!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -32628,9 +32628,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27)+27,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,28)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*28+27),"dd mmmm yyyy"))</f>
         <v>11 July 2027 - 10 August 2027</v>
       </c>
-      <c r="J30" s="141" t="e">
+      <c r="J30" s="141">
         <f ca="1">Forecast_10!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -32638,9 +32638,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,28),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*28)+28,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,29)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*29+28),"dd mmmm yyyy"))</f>
         <v>11 August 2027 - 10 September 2027</v>
       </c>
-      <c r="J31" s="139" t="e">
+      <c r="J31" s="139">
         <f ca="1">Forecast_10!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -32648,9 +32648,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,29),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*29)+29,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
         <v>11 September 2027 - 10 October 2027</v>
       </c>
-      <c r="J32" s="139" t="e">
+      <c r="J32" s="139">
         <f ca="1">Forecast_10!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -32658,9 +32658,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30)+30,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,31)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*31+30),"dd mmmm yyyy"))</f>
         <v>11 October 2027 - 10 November 2027</v>
       </c>
-      <c r="J33" s="139" t="e">
+      <c r="J33" s="139">
         <f ca="1">Forecast_11!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -32678,9 +32678,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,31),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*31)+31,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,32)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*32+31),"dd mmmm yyyy"))</f>
         <v>11 November 2027 - 10 December 2027</v>
       </c>
-      <c r="J34" s="139" t="e">
+      <c r="J34" s="139">
         <f ca="1">Forecast_11!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -32703,9 +32703,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,32),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*32)+32,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
         <v>11 December 2027 - 10 January 2028</v>
       </c>
-      <c r="J35" s="139" t="e">
+      <c r="J35" s="139">
         <f ca="1">Forecast_11!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -32722,9 +32722,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33)+33,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,34)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*34+33),"dd mmmm yyyy"))</f>
         <v>11 January 2028 - 10 February 2028</v>
       </c>
-      <c r="J36" s="139" t="e">
+      <c r="J36" s="139">
         <f ca="1">Forecast_12!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -32741,9 +32741,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,34),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*34)+34,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,35)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*35+34),"dd mmmm yyyy"))</f>
         <v>11 February 2028 - 10 March 2028</v>
       </c>
-      <c r="J37" s="139" t="e">
+      <c r="J37" s="139">
         <f ca="1">Forecast_12!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -32760,9 +32760,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,35),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*35)+35,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
         <v>11 March 2028 - 10 April 2028</v>
       </c>
-      <c r="J38" s="139" t="e">
+      <c r="J38" s="139">
         <f ca="1">Forecast_12!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -32779,9 +32779,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36)+36,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,37)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*37+36),"dd mmmm yyyy"))</f>
         <v>11 April 2028 - 10 May 2028</v>
       </c>
-      <c r="J39" s="139" t="e">
+      <c r="J39" s="139">
         <f ca="1">Forecast_13!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -32798,9 +32798,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,37),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*37)+37,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,38)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*38+37),"dd mmmm yyyy"))</f>
         <v>11 May 2028 - 10 June 2028</v>
       </c>
-      <c r="J40" s="139" t="e">
+      <c r="J40" s="139">
         <f ca="1">Forecast_13!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -32817,9 +32817,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,38),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*38)+38,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
         <v>11 June 2028 - 10 July 2028</v>
       </c>
-      <c r="J41" s="139" t="e">
+      <c r="J41" s="139">
         <f ca="1">Forecast_13!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -32839,9 +32839,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39)+39,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,40)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*40+39),"dd mmmm yyyy"))</f>
         <v>11 July 2028 - 10 August 2028</v>
       </c>
-      <c r="J42" s="139" t="e">
+      <c r="J42" s="139">
         <f ca="1">Forecast_14!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -32849,9 +32849,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,40),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*40)+40,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,41)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*41+40),"dd mmmm yyyy"))</f>
         <v>11 August 2028 - 10 September 2028</v>
       </c>
-      <c r="J43" s="139" t="e">
+      <c r="J43" s="139">
         <f ca="1">Forecast_14!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -32859,9 +32859,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,41),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*41)+41,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
         <v>11 September 2028 - 10 October 2028</v>
       </c>
-      <c r="J44" s="139" t="e">
+      <c r="J44" s="139">
         <f ca="1">Forecast_14!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -32869,9 +32869,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42)+42,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,43)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*43+42),"dd mmmm yyyy"))</f>
         <v>11 October 2028 - 10 November 2028</v>
       </c>
-      <c r="J45" s="139" t="e">
+      <c r="J45" s="139">
         <f ca="1">Forecast_15!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -32889,9 +32889,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,43),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*43)+43,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,44)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*44+43),"dd mmmm yyyy"))</f>
         <v>11 November 2028 - 10 December 2028</v>
       </c>
-      <c r="J46" s="139" t="e">
+      <c r="J46" s="139">
         <f ca="1">Forecast_15!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -32914,9 +32914,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,44),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*44)+44,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
         <v>11 December 2028 - 10 January 2029</v>
       </c>
-      <c r="J47" s="139" t="e">
+      <c r="J47" s="139">
         <f ca="1">Forecast_15!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -32933,9 +32933,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45)+45,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,46)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*46+45),"dd mmmm yyyy"))</f>
         <v>11 January 2029 - 10 February 2029</v>
       </c>
-      <c r="J48" s="139" t="e">
+      <c r="J48" s="139">
         <f ca="1">Forecast_16!E136</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -32952,9 +32952,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,46),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*46)+46,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,47)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*47+46),"dd mmmm yyyy"))</f>
         <v>11 February 2029 - 10 March 2029</v>
       </c>
-      <c r="J49" s="139" t="e">
+      <c r="J49" s="139">
         <f ca="1">Forecast_16!E163</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -32971,9 +32971,9 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,47),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*47)+47,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
         <v>11 March 2029 - 10 April 2029</v>
       </c>
-      <c r="J50" s="135" t="e">
+      <c r="J50" s="135">
         <f ca="1">Forecast_16!E190</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" ht="24.75" customHeight="1" spans="1:7">
@@ -37308,7 +37308,7 @@
     </row>
     <row r="193" s="43" customFormat="1" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -40295,7 +40295,7 @@
     </row>
     <row r="192" ht="30" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -43301,7 +43301,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G29" name="R2"/>
@@ -46324,7 +46324,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -49345,7 +49345,7 @@
       <c r="I193" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -49763,7 +49763,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121"/>
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>

</xml_diff>

<commit_message>
docs: 1. Fix the Overall Total for each forecast.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4140,8 +4140,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -4174,7 +4174,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -7162,8 +7162,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -7196,7 +7196,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -10184,8 +10184,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -10219,7 +10219,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -13207,8 +13207,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -13240,7 +13240,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -16228,8 +16228,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -16263,7 +16263,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -19251,8 +19251,8 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -19284,7 +19284,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -22273,8 +22273,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -22306,7 +22306,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -25294,8 +25294,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -25327,7 +25327,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -28315,8 +28315,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G116" sqref="G116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -28350,7 +28350,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -31886,8 +31886,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34727,8 +34727,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34762,7 +34762,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -37716,8 +37716,8 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37749,7 +37749,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -40696,8 +40696,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -40730,7 +40730,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -43718,8 +43718,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -43753,7 +43753,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -46741,8 +46741,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46774,7 +46774,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>
@@ -49762,8 +49762,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -49795,7 +49795,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
         <v>0</v>
       </c>
       <c r="D2" s="4"/>

</xml_diff>

<commit_message>
docs: 1. Fix the calculation for the forecasts in worksheet 1.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560"/>
+    <workbookView windowHeight="21560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -81,7 +81,8 @@
     <t>tens</t>
   </si>
   <si>
-    <t>A Month</t>
+    <t>A Month
+TRUE or FALSE</t>
   </si>
   <si>
     <t>Date Range Start From
@@ -2404,8 +2405,8 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC36" sqref="AC36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="17.6"/>
@@ -4166,7 +4167,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
@@ -34074,8 +34075,8 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
@@ -34622,8 +34623,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B79" sqref="A71:B79"/>
+    <sheetView topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="E203" sqref="E203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36832,7 +36833,7 @@
       </c>
       <c r="D176" s="81"/>
       <c r="E176" s="90">
-        <f>(F42+E156)-(SUM(E159:E167)+SUM(E169:E175))</f>
+        <f>(F42+E156)-(SUM(E158:E167)+SUM(E169:E175))</f>
         <v>0</v>
       </c>
     </row>
@@ -37087,7 +37088,7 @@
       </c>
       <c r="D203" s="81"/>
       <c r="E203" s="90">
-        <f>(F54+E183)-(SUM(E189:E194)+SUM(E196:E202))</f>
+        <f>(F54+E183)-(SUM(E185:E194)+SUM(E196:E202))</f>
         <v>0</v>
       </c>
     </row>
@@ -37495,8 +37496,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>

</xml_diff>

<commit_message>
docs: 1. Fix the bug of handling debts for the second worksheet.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -34623,8 +34623,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="E203" sqref="E203"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37496,8 +37496,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -39082,7 +39082,7 @@
         <v/>
       </c>
       <c r="C99" s="95" cm="1">
-        <f ca="1" t="array" ref="C99">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E132")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E159")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E186")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C113")</f>
+        <f ca="1" t="array" ref="C99">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E132")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E159")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E186")))+SUM(E119+E146+E173))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C113")</f>
         <v>0</v>
       </c>
       <c r="D99" s="14"/>
@@ -39102,7 +39102,7 @@
         <v/>
       </c>
       <c r="C100" s="95" cm="1">
-        <f ca="1" t="array" ref="C100">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E133")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E160")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E187")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C114")</f>
+        <f ca="1" t="array" ref="C100">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E133")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E160")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E187")))+SUM(E120+E147+E174))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C114")</f>
         <v>0</v>
       </c>
       <c r="D100" s="14"/>
@@ -39122,7 +39122,7 @@
         <v/>
       </c>
       <c r="C101" s="95" cm="1">
-        <f ca="1" t="array" ref="C101">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E134")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E161")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E188")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C115")</f>
+        <f ca="1" t="array" ref="C101">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E134")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E161")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E188")))+SUM(E121+E148+E175))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C115")</f>
         <v>0</v>
       </c>
       <c r="D101" s="14"/>
@@ -39142,7 +39142,7 @@
         <v/>
       </c>
       <c r="C102" s="95" cm="1">
-        <f ca="1" t="array" ref="C102">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E135")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E162")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E189")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C116")</f>
+        <f ca="1" t="array" ref="C102">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E135")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E162")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E189")))+SUM(E122+E149+E176))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C116")</f>
         <v>0</v>
       </c>
       <c r="D102" s="14"/>
@@ -39162,7 +39162,7 @@
         <v/>
       </c>
       <c r="C103" s="95" cm="1">
-        <f ca="1" t="array" ref="C103">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E136")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E163")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E190")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C117")</f>
+        <f ca="1" t="array" ref="C103">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E136")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E163")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E190")))+SUM(EE123+E150+E177)-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C117"))</f>
         <v>0</v>
       </c>
       <c r="D103" s="14"/>
@@ -39182,7 +39182,7 @@
         <v/>
       </c>
       <c r="C104" s="95" cm="1">
-        <f ca="1" t="array" ref="C104">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E137")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E164")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E191")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C118")</f>
+        <f ca="1" t="array" ref="C104">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E137")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E164")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E191")))+SUM(E124+E151+E178))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C118")</f>
         <v>0</v>
       </c>
       <c r="D104" s="14"/>
@@ -39202,7 +39202,7 @@
         <v/>
       </c>
       <c r="C105" s="95" cm="1">
-        <f ca="1" t="array" ref="C105">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E138")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E165")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E192")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C119")</f>
+        <f ca="1" t="array" ref="C105">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E138")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E165")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E192")))+SUM(E125+E152+E179)-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C119"))</f>
         <v>0</v>
       </c>
       <c r="D105" s="14"/>
@@ -39222,7 +39222,7 @@
         <v/>
       </c>
       <c r="C106" s="95" cm="1">
-        <f ca="1" t="array" ref="C106">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E139")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E166")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E193")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C120")</f>
+        <f ca="1" t="array" ref="C106">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E139")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E166")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E193")))+SUM(E126+E153+E180))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C120")</f>
         <v>0</v>
       </c>
       <c r="D106" s="14"/>
@@ -39242,7 +39242,7 @@
         <v/>
       </c>
       <c r="C107" s="95" cm="1">
-        <f ca="1" t="array" ref="C107">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E140")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E167")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E194")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C121")</f>
+        <f ca="1" t="array" ref="C107">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E140")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E167")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E194")))+SUM(E127+E154+E181))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C121")</f>
         <v>0</v>
       </c>
       <c r="D107" s="14"/>
@@ -40787,8 +40787,8 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -43666,7 +43666,7 @@
     </row>
     <row r="192" ht="30" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -47393,8 +47393,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>

</xml_diff>

<commit_message>
docs: 1. Protect un-protect worksheet. 2. Switch to the Cover page.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="3"/>
+    <workbookView windowHeight="21560"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -2405,7 +2405,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
@@ -4168,7 +4168,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -7492,7 +7492,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -10816,7 +10816,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -14141,7 +14141,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -17464,7 +17464,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -20789,7 +20789,7 @@
   <dimension ref="A1:I194"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -24113,7 +24113,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -27436,7 +27436,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -30760,7 +30760,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34076,7 +34076,7 @@
   <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
@@ -34587,7 +34587,7 @@
     <row r="133" s="152" customFormat="1" ht="20.25" customHeight="1"/>
     <row r="134" s="152" customFormat="1" ht="20.25" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0"/>
+  <sheetProtection sheet="1" formatCells="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="B1:B6" name="Settings"/>
     <protectedRange sqref="B9:B56" name="NameOfWorkSheet"/>
@@ -37496,8 +37496,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -40788,7 +40788,7 @@
   <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -43666,7 +43666,7 @@
     </row>
     <row r="192" ht="30" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15" name="R1"/>
     <protectedRange sqref="A22:G27" name="R2"/>
@@ -44070,7 +44070,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -47394,7 +47394,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50719,7 +50719,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -54042,7 +54042,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>

</xml_diff>

<commit_message>
docs: 1.Protect Worksheet. 2. Switch to cover page.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -2254,7 +2254,7 @@
     <cellStyle name="Revenue Header Font" xfId="53"/>
     <cellStyle name="Total Label" xfId="54"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="7">
     <dxf>
       <font>
         <color theme="3" tint="0.5"/>
@@ -2296,36 +2296,6 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF5B9BD5"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -7323,7 +7293,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -7504,10 +7474,10 @@
     <mergeCell ref="A171:B188"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7528,10 +7498,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="32" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="31" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="32" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="31" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7648,15 +7618,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="30" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="30" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="29" operator="greaterThan">
@@ -7664,7 +7634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -7672,7 +7642,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -7698,12 +7668,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="39" operator="greaterThan">
@@ -10632,7 +10602,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -10813,10 +10783,10 @@
     <mergeCell ref="A171:B188"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10837,10 +10807,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10957,15 +10927,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -10973,7 +10943,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -10981,7 +10951,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -11007,12 +10977,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -13943,7 +13913,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -14124,10 +14094,10 @@
     <mergeCell ref="A171:B188"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14148,10 +14118,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14268,15 +14238,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -14284,7 +14254,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -14292,7 +14262,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -14318,12 +14288,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -17251,7 +17221,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -17432,10 +17402,10 @@
     <mergeCell ref="A171:B188"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17456,10 +17426,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17576,15 +17546,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -17592,7 +17562,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -17600,7 +17570,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -17626,12 +17596,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -20562,7 +20532,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -20743,10 +20713,10 @@
     <mergeCell ref="A171:B188"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20767,10 +20737,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20887,15 +20857,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -20903,7 +20873,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -20911,7 +20881,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -20937,12 +20907,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -20959,7 +20929,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
@@ -23871,7 +23841,7 @@
     </row>
     <row r="194" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C98:C107 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -24052,10 +24022,10 @@
     <mergeCell ref="A117:B134"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24076,10 +24046,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24196,15 +24166,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -24212,7 +24182,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -24220,7 +24190,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -24246,12 +24216,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -27179,7 +27149,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C98:C107 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -27360,10 +27330,10 @@
     <mergeCell ref="A117:B134"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27384,10 +27354,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27504,15 +27474,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -27520,7 +27490,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -27528,7 +27498,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -27554,12 +27524,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -27576,7 +27546,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
@@ -30487,7 +30457,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C98:C107 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -30668,10 +30638,10 @@
     <mergeCell ref="A117:B134"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30692,10 +30662,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30812,15 +30782,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -30828,7 +30798,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -30836,7 +30806,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -30862,12 +30832,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -33798,7 +33768,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -33979,10 +33949,10 @@
     <mergeCell ref="A117:B134"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34003,10 +33973,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="29" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="28" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="29" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="28" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34123,15 +34093,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="27" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="27" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="26" operator="greaterThan">
@@ -34139,7 +34109,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -34147,7 +34117,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -34173,12 +34143,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="36" operator="greaterThan">
@@ -37182,7 +37152,7 @@
     </row>
     <row r="204" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="C3:C15 F3:F15 A24:G29 A36:G41 A48:G53 A61:C68 A71:C79 A82:C88 A91:C98 A101:C108 A112:C121 C131:E140 C142:E147 C158:E167 C185:E194 C196:E201" name="Values"/>
     <protectedRange sqref="B3:B15 E3:E15" name="Label"/>
@@ -37502,7 +37472,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131:E140">
-    <cfRule type="cellIs" dxfId="5" priority="29" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="29" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="28" operator="greaterThan">
@@ -37510,7 +37480,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158:E167">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
@@ -37518,7 +37488,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185:E194">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -37526,12 +37496,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J50">
-    <cfRule type="cellIs" dxfId="6" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="23" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N18">
-    <cfRule type="cellIs" dxfId="7" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37557,7 +37527,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E157 E168:E175">
-    <cfRule type="cellIs" dxfId="6" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="44" operator="greaterThan">
@@ -37565,7 +37535,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E184 E195:E202">
-    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="36" operator="greaterThan">
@@ -40469,7 +40439,7 @@
     </row>
     <row r="193" s="44" customFormat="1" ht="24.75" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -40650,10 +40620,10 @@
     <mergeCell ref="A117:B134"/>
   </mergeCells>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="7" priority="29" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="28" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="29" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="28" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40674,10 +40644,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="9" priority="27" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="27" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40786,15 +40756,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="25" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="25" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="24" operator="greaterThan">
@@ -40802,7 +40772,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="9" operator="greaterThan">
@@ -40810,7 +40780,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
@@ -40836,12 +40806,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="34" operator="greaterThan">
@@ -43743,7 +43713,7 @@
     </row>
     <row r="192" ht="30" customHeight="1"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -43948,10 +43918,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="9" priority="28" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="28" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43980,7 +43950,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E154">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
@@ -44060,15 +44030,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -44076,7 +44046,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E153">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="9" operator="greaterThan">
@@ -44084,7 +44054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -44110,12 +44080,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -47249,10 +47219,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="24" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="24" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="23" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47369,15 +47339,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="21" operator="greaterThan">
@@ -47385,7 +47355,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -47393,7 +47363,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
@@ -47419,12 +47389,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="31" operator="greaterThan">
@@ -50355,7 +50325,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -50560,10 +50530,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="30" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="30" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="29" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50680,15 +50650,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="28" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="28" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="27" operator="greaterThan">
@@ -50696,7 +50666,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
@@ -50704,7 +50674,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -50730,12 +50700,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="43" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="37" operator="greaterThan">
@@ -53663,7 +53633,7 @@
       <c r="I193" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C84 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -53868,10 +53838,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="8" priority="28" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="28" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53988,15 +53958,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -54004,7 +53974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -54012,7 +53982,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -54038,12 +54008,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">
@@ -56970,7 +56940,7 @@
       <c r="I193" s="126"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A10:G15 A22:G27 A34:G39 C47:C54 C57:C65 C68:C74 C77:C83 C87:C94 C118:E127 C129:E134 C145:E154 C156:E161 C172:E181 C183:E188" name="Values"/>
   </protectedRanges>
@@ -57175,10 +57145,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="7" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -57295,15 +57265,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C109">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E118:E127">
-    <cfRule type="cellIs" dxfId="5" priority="26" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="25" operator="greaterThan">
@@ -57311,7 +57281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:E154">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
@@ -57319,7 +57289,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E172:E181">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
@@ -57345,12 +57315,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144 E155:E162">
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E171 E182:E189">
-    <cfRule type="cellIs" dxfId="6" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="35" operator="greaterThan">

</xml_diff>

<commit_message>
docs: 1. Deferred the payback debt for Mom.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast Template.xlsx
+++ b/Income And Expenses Forecast Template.xlsx
@@ -34739,8 +34739,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37599,7 +37599,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
@@ -40876,7 +40876,7 @@
   <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>

</xml_diff>